<commit_message>
Done due date set up
</commit_message>
<xml_diff>
--- a/List WIP.xlsx
+++ b/List WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GAD_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77FDA8B-7AC0-4E19-A287-A78823C55E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2733BCF-9701-4565-BB7E-221A8A6788E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>Number</t>
   </si>
@@ -581,8 +581,8 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +894,10 @@
         <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
@@ -908,7 +911,10 @@
         <v>41</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">

</xml_diff>